<commit_message>
Added documenation, some extra tests, and updated the main program.
I also fixed a bug with the red-black tree and a bug with counting data. Estimated time 1 hour.
</commit_message>
<xml_diff>
--- a/src/countMeetings/csv-files/CountChecker.xlsx
+++ b/src/countMeetings/csv-files/CountChecker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexl\eclipse-workspace\CalendarApp\src\countMeetings\csv-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Interviews\raytheon-practice\CalendarApp\src\countMeetings\csv-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CF84CE-0131-4F51-B98D-CD392E60F7B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D74AE7F-20C5-4521-99B3-836624AB2121}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5738" yWindow="690" windowWidth="12202" windowHeight="9533" xr2:uid="{BED3BC06-C2A8-4C98-933F-1C2931D03933}"/>
+    <workbookView minimized="1" xWindow="3410" yWindow="4520" windowWidth="17240" windowHeight="15460" xr2:uid="{BED3BC06-C2A8-4C98-933F-1C2931D03933}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,14 +31,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -431,16 +429,18 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" customWidth="1"/>
+    <col min="5" max="5" width="23.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43222</v>
       </c>
@@ -479,7 +479,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>

</xml_diff>